<commit_message>
Changes in selected file
</commit_message>
<xml_diff>
--- a/files/reporteMensual_Excel.xlsx
+++ b/files/reporteMensual_Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Todo\Documentos\Santiago\3_Trabajo Profesional\Full-Stack-Projects\Bodega\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bodega\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF8E4412-E6DE-4C02-A316-FB16FB062B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5CAF26BA-18B7-416D-B16B-A1FCED0204DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="reporteMensual_Excel" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1757" uniqueCount="872">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1759" uniqueCount="873">
   <si>
     <t>Cï¿½digo prestador</t>
   </si>
@@ -2651,11 +2651,14 @@
   <si>
     <t>320 644 89 43</t>
   </si>
+  <si>
+    <t>Bogota</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3493,10 +3496,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EU137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -9759,7 +9764,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="15" spans="1:151" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:151" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>22103</v>
       </c>
@@ -12008,6 +12013,9 @@
       <c r="F20" t="s">
         <v>280</v>
       </c>
+      <c r="G20" t="s">
+        <v>872</v>
+      </c>
       <c r="H20" t="s">
         <v>154</v>
       </c>
@@ -20897,7 +20905,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="40" spans="1:151" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:151" ht="75" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>22106</v>
       </c>
@@ -30215,7 +30223,7 @@
         <v>3015869922</v>
       </c>
     </row>
-    <row r="61" spans="1:151" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:151" ht="150" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>22031</v>
       </c>
@@ -30677,6 +30685,9 @@
       <c r="G62" t="s">
         <v>153</v>
       </c>
+      <c r="H62" t="s">
+        <v>154</v>
+      </c>
       <c r="I62" t="s">
         <v>516</v>
       </c>
@@ -31095,7 +31106,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="63" spans="1:151" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:151" ht="360" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>22158</v>
       </c>
@@ -54218,7 +54229,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="115" spans="1:151" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:151" ht="210" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>22117</v>
       </c>

</xml_diff>

<commit_message>
New consolidado card with their info
</commit_message>
<xml_diff>
--- a/files/reporteMensual_Excel.xlsx
+++ b/files/reporteMensual_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bodega\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5CAF26BA-18B7-416D-B16B-A1FCED0204DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D5B3BECD-39D5-49CB-ADAA-188E40DCDDA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2795,7 +2795,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2975,6 +2975,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -3136,12 +3142,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3499,11 +3506,18 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EU137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3533,7 +3547,7 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K1" t="s">
@@ -3542,7 +3556,7 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="N1" t="s">
@@ -3551,7 +3565,7 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="Q1" t="s">

</xml_diff>